<commit_message>
adapting excel and script after thesis meeting
creating bar charts for coefficients (absolute values for now)
</commit_message>
<xml_diff>
--- a/data/meta_model/m1.covar.xlsx
+++ b/data/meta_model/m1.covar.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t xml:space="preserve">ind_code</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t xml:space="preserve">others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bulk desity</t>
   </si>
   <si>
     <t xml:space="preserve">soil ph</t>
@@ -4147,10 +4144,10 @@
         <v>121</v>
       </c>
       <c r="I128" t="n">
-        <v>1.59517901453385</v>
+        <v>1.52747340063067</v>
       </c>
       <c r="J128" t="n">
-        <v>14.4649446494464</v>
+        <v>14.1310952694971</v>
       </c>
     </row>
     <row r="129">
@@ -4175,10 +4172,10 @@
         <v>121</v>
       </c>
       <c r="I129" t="n">
-        <v>1.59517901453385</v>
+        <v>1.32803247853033</v>
       </c>
       <c r="J129" t="n">
-        <v>14.4649446494464</v>
+        <v>9.56229667740116</v>
       </c>
     </row>
     <row r="130">
@@ -4203,10 +4200,10 @@
         <v>145</v>
       </c>
       <c r="I130" t="n">
-        <v>1.39261659998987</v>
+        <v>1.33665357744385</v>
       </c>
       <c r="J130" t="n">
-        <v>17.1217712177121</v>
+        <v>16.4504593125411</v>
       </c>
     </row>
     <row r="131">
@@ -4231,10 +4228,10 @@
         <v>145</v>
       </c>
       <c r="I131" t="n">
-        <v>1.39261659998987</v>
+        <v>1.37608774204019</v>
       </c>
       <c r="J131" t="n">
-        <v>17.1217712177121</v>
+        <v>17.3220353627825</v>
       </c>
     </row>
     <row r="132">
@@ -14210,7 +14207,7 @@
         <v>47</v>
       </c>
       <c r="B454" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C454" t="s">
         <v>19</v>
@@ -14227,10 +14224,10 @@
         <v>8</v>
       </c>
       <c r="I454" t="n">
-        <v>5.29918304261426</v>
+        <v>1.52747340063067</v>
       </c>
       <c r="J454" t="n">
-        <v>10.4468412942989</v>
+        <v>14.1310952694971</v>
       </c>
     </row>
     <row r="455">
@@ -14238,7 +14235,7 @@
         <v>47</v>
       </c>
       <c r="B455" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C455" t="s">
         <v>20</v>
@@ -14255,10 +14252,10 @@
         <v>31</v>
       </c>
       <c r="I455" t="n">
-        <v>2.39724947165883</v>
+        <v>1.32803247853033</v>
       </c>
       <c r="J455" t="n">
-        <v>-1.51001540832049</v>
+        <v>9.56229667740116</v>
       </c>
     </row>
     <row r="456">
@@ -14266,7 +14263,7 @@
         <v>47</v>
       </c>
       <c r="B456" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C456" t="s">
         <v>21</v>
@@ -14283,10 +14280,10 @@
         <v>12</v>
       </c>
       <c r="I456" t="n">
-        <v>4.76295618711163</v>
+        <v>1.33665357744385</v>
       </c>
       <c r="J456" t="n">
-        <v>8.59784283513097</v>
+        <v>16.4504593125411</v>
       </c>
     </row>
     <row r="457">
@@ -14294,7 +14291,7 @@
         <v>47</v>
       </c>
       <c r="B457" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C457" t="s">
         <v>22</v>
@@ -14311,15 +14308,15 @@
         <v>6</v>
       </c>
       <c r="I457" t="n">
-        <v>8.95814276251459</v>
+        <v>1.37608774204019</v>
       </c>
       <c r="J457" t="n">
-        <v>25.6086286594761</v>
+        <v>17.3220353627825</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B458" t="s">
         <v>50</v>
@@ -14347,7 +14344,7 @@
     </row>
     <row r="459">
       <c r="A459" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B459" t="s">
         <v>50</v>
@@ -14375,7 +14372,7 @@
     </row>
     <row r="460">
       <c r="A460" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B460" t="s">
         <v>50</v>
@@ -14403,7 +14400,7 @@
     </row>
     <row r="461">
       <c r="A461" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B461" t="s">
         <v>23</v>
@@ -14431,7 +14428,7 @@
     </row>
     <row r="462">
       <c r="A462" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B462" t="s">
         <v>23</v>
@@ -14459,7 +14456,7 @@
     </row>
     <row r="463">
       <c r="A463" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B463" t="s">
         <v>23</v>
@@ -14487,7 +14484,7 @@
     </row>
     <row r="464">
       <c r="A464" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B464" t="s">
         <v>23</v>
@@ -14515,7 +14512,7 @@
     </row>
     <row r="465">
       <c r="A465" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B465" t="s">
         <v>23</v>
@@ -14543,7 +14540,7 @@
     </row>
     <row r="466">
       <c r="A466" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B466" t="s">
         <v>23</v>
@@ -14571,13 +14568,13 @@
     </row>
     <row r="467">
       <c r="A467" t="s">
+        <v>69</v>
+      </c>
+      <c r="B467" t="s">
+        <v>25</v>
+      </c>
+      <c r="C467" t="s">
         <v>70</v>
-      </c>
-      <c r="B467" t="s">
-        <v>25</v>
-      </c>
-      <c r="C467" t="s">
-        <v>71</v>
       </c>
       <c r="D467"/>
       <c r="E467"/>
@@ -14599,13 +14596,13 @@
     </row>
     <row r="468">
       <c r="A468" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B468" t="s">
         <v>25</v>
       </c>
       <c r="C468" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D468"/>
       <c r="E468"/>
@@ -14627,13 +14624,13 @@
     </row>
     <row r="469">
       <c r="A469" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B469" t="s">
         <v>25</v>
       </c>
       <c r="C469" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D469"/>
       <c r="E469"/>
@@ -14655,10 +14652,10 @@
     </row>
     <row r="470">
       <c r="A470" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B470" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C470" t="s">
         <v>31</v>
@@ -14683,10 +14680,10 @@
     </row>
     <row r="471">
       <c r="A471" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B471" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C471" t="s">
         <v>31</v>
@@ -14711,10 +14708,10 @@
     </row>
     <row r="472">
       <c r="A472" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B472" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C472" t="s">
         <v>31</v>
@@ -14739,10 +14736,10 @@
     </row>
     <row r="473">
       <c r="A473" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B473" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C473" t="s">
         <v>31</v>
@@ -14767,10 +14764,10 @@
     </row>
     <row r="474">
       <c r="A474" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B474" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C474" t="s">
         <v>31</v>
@@ -14795,7 +14792,7 @@
     </row>
     <row r="475">
       <c r="A475" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B475" t="s">
         <v>34</v>
@@ -14823,7 +14820,7 @@
     </row>
     <row r="476">
       <c r="A476" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B476" t="s">
         <v>34</v>
@@ -14851,7 +14848,7 @@
     </row>
     <row r="477">
       <c r="A477" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B477" t="s">
         <v>34</v>
@@ -14879,7 +14876,7 @@
     </row>
     <row r="478">
       <c r="A478" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B478" t="s">
         <v>34</v>
@@ -14907,7 +14904,7 @@
     </row>
     <row r="479">
       <c r="A479" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B479" t="s">
         <v>34</v>
@@ -15193,7 +15190,7 @@
         <v>25</v>
       </c>
       <c r="C489" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D489"/>
       <c r="E489"/>
@@ -15221,7 +15218,7 @@
         <v>25</v>
       </c>
       <c r="C490" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D490"/>
       <c r="E490"/>
@@ -15249,7 +15246,7 @@
         <v>25</v>
       </c>
       <c r="C491" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D491"/>
       <c r="E491"/>
@@ -15274,7 +15271,7 @@
         <v>10</v>
       </c>
       <c r="B492" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C492" t="s">
         <v>31</v>
@@ -15302,7 +15299,7 @@
         <v>10</v>
       </c>
       <c r="B493" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C493" t="s">
         <v>31</v>
@@ -15330,7 +15327,7 @@
         <v>10</v>
       </c>
       <c r="B494" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C494" t="s">
         <v>31</v>
@@ -15358,7 +15355,7 @@
         <v>10</v>
       </c>
       <c r="B495" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C495" t="s">
         <v>31</v>
@@ -15386,7 +15383,7 @@
         <v>10</v>
       </c>
       <c r="B496" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C496" t="s">
         <v>31</v>
@@ -15548,18 +15545,6 @@
       <c r="J501" t="n">
         <v>10.3241396696846</v>
       </c>
-    </row>
-    <row r="502">
-      <c r="A502"/>
-      <c r="B502"/>
-      <c r="C502"/>
-      <c r="D502"/>
-      <c r="E502"/>
-      <c r="F502"/>
-      <c r="G502"/>
-      <c r="H502"/>
-      <c r="I502"/>
-      <c r="J502"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>